<commit_message>
suite dev fns utilisateur
</commit_message>
<xml_diff>
--- a/utilisateurs/utilisateurs.xlsx
+++ b/utilisateurs/utilisateurs.xlsx
@@ -1,72 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcvou\Dropbox\AA-Perso\Anaconda-Python38-spyder\memolab\utilisateurs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9732C724-B8FD-4693-B886-1C5971A9BF37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{19604962-0A62-4731-887B-EDA0C03033B9}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>numPos</t>
-  </si>
-  <si>
-    <t>nomUtilisateur</t>
-  </si>
-  <si>
-    <t>fichierUtilisateur</t>
-  </si>
-  <si>
-    <t>Jean-Claude Vouillamoz</t>
-  </si>
-  <si>
-    <t>jeanclaudevouillamoz.xlsx</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -105,26 +66,86 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{DA11CDFF-3AA7-43E9-A8B4-087A3FB97B60}"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0"/>
   </tableStyles>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -424,130 +445,242 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{196DDB7A-1F75-4C59-AD24-B0605A7662A4}">
-  <dimension ref="A1:C20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="32.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.5546875" customWidth="1"/>
+    <col width="32.33203125" customWidth="1" min="3" max="3"/>
+    <col width="30.5546875" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>numPos</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>pseudo</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>prenomNom</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>fichierUtilisateur</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>jcv</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>Jean-Claude Vouillamoz</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>jeanclaudevouillamoz.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>dama</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>Damaris Fontaine</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>damarisfontaine.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Lucien</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>Lucien Vouillamoz</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>lucienvouillamoz.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>SuzVou</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>Suzanne Vouillamoz</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>suzannevouillamoz.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>àüöro</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>öüäéèà</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>SuzLys</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>SuzLys V</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>suzlysv.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="n"/>
+      <c r="B8" s="3" t="n"/>
+      <c r="C8" s="3" t="n"/>
+      <c r="D8" s="3" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="n"/>
+      <c r="B9" s="3" t="n"/>
+      <c r="C9" s="3" t="n"/>
+      <c r="D9" s="3" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n"/>
+      <c r="B10" s="3" t="n"/>
+      <c r="C10" s="3" t="n"/>
+      <c r="D10" s="3" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n"/>
+      <c r="B11" s="3" t="n"/>
+      <c r="C11" s="3" t="n"/>
+      <c r="D11" s="3" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n"/>
+      <c r="B12" s="3" t="n"/>
+      <c r="C12" s="3" t="n"/>
+      <c r="D12" s="3" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="n"/>
+      <c r="B13" s="3" t="n"/>
+      <c r="C13" s="3" t="n"/>
+      <c r="D13" s="3" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="n"/>
+      <c r="B14" s="3" t="n"/>
+      <c r="C14" s="3" t="n"/>
+      <c r="D14" s="3" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="n"/>
+      <c r="B15" s="3" t="n"/>
+      <c r="C15" s="3" t="n"/>
+      <c r="D15" s="3" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="n"/>
+      <c r="B16" s="3" t="n"/>
+      <c r="C16" s="3" t="n"/>
+      <c r="D16" s="3" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="n"/>
+      <c r="B17" s="3" t="n"/>
+      <c r="C17" s="3" t="n"/>
+      <c r="D17" s="3" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="n"/>
+      <c r="B18" s="3" t="n"/>
+      <c r="C18" s="3" t="n"/>
+      <c r="D18" s="3" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="n"/>
+      <c r="B19" s="3" t="n"/>
+      <c r="C19" s="3" t="n"/>
+      <c r="D19" s="3" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="n"/>
+      <c r="B20" s="3" t="n"/>
+      <c r="C20" s="3" t="n"/>
+      <c r="D20" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>